<commit_message>
Added talkboack notes and split position
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24181059-2C31-450E-8FAA-E8C56745C15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4F7900-3082-402E-AB6A-F85CE2116DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="120">
   <si>
     <t>Input</t>
   </si>
@@ -323,6 +323,81 @@
   </si>
   <si>
     <t>John IEM</t>
+  </si>
+  <si>
+    <t>Talkback is on port 12 of the bottom splitter</t>
+  </si>
+  <si>
+    <t>Top 1</t>
+  </si>
+  <si>
+    <t>Top 2</t>
+  </si>
+  <si>
+    <t>Top 3</t>
+  </si>
+  <si>
+    <t>Top 4</t>
+  </si>
+  <si>
+    <t>Top 5</t>
+  </si>
+  <si>
+    <t>Top 6</t>
+  </si>
+  <si>
+    <t>Top 7</t>
+  </si>
+  <si>
+    <t>Top 8</t>
+  </si>
+  <si>
+    <t>Top 9</t>
+  </si>
+  <si>
+    <t>Top 10</t>
+  </si>
+  <si>
+    <t>Top 11</t>
+  </si>
+  <si>
+    <t>Top 12</t>
+  </si>
+  <si>
+    <t>Top 13</t>
+  </si>
+  <si>
+    <t>Top 14</t>
+  </si>
+  <si>
+    <t>Top 15</t>
+  </si>
+  <si>
+    <t>Top 16</t>
+  </si>
+  <si>
+    <t>Bottom 1</t>
+  </si>
+  <si>
+    <t>Bottom 2</t>
+  </si>
+  <si>
+    <t>Bottom 3</t>
+  </si>
+  <si>
+    <t>Bottom 4</t>
+  </si>
+  <si>
+    <t>Bottom 5</t>
+  </si>
+  <si>
+    <t>Bottom 6</t>
+  </si>
+  <si>
+    <t>Bottom 7</t>
+  </si>
+  <si>
+    <t>Bottom 8</t>
   </si>
 </sst>
 </file>
@@ -635,7 +710,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -772,11 +847,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -819,6 +909,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -906,6 +998,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,46 +1016,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1136,9 +1213,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1176,7 +1253,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1282,7 +1359,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1424,7 +1501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1434,25 +1511,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" customWidth="1"/>
-    <col min="2" max="2" width="7.54296875" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="22" width="7.26953125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="22" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>56</v>
       </c>
@@ -1481,11 +1558,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="4">
@@ -1508,9 +1585,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="5">
         <v>2</v>
       </c>
@@ -1529,9 +1606,9 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="4">
         <v>3</v>
       </c>
@@ -1554,9 +1631,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
@@ -1579,9 +1656,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>5</v>
       </c>
@@ -1604,9 +1681,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="5">
         <v>6</v>
       </c>
@@ -1629,9 +1706,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
@@ -1654,9 +1731,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
@@ -1679,9 +1756,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4">
         <v>9</v>
       </c>
@@ -1704,60 +1781,60 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4">
         <v>11</v>
       </c>
       <c r="D12" s="26">
         <v>11</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="5">
         <v>12</v>
       </c>
       <c r="D13" s="27">
         <v>12</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="44"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="4">
         <v>13</v>
       </c>
@@ -1776,9 +1853,9 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="5">
         <v>14</v>
       </c>
@@ -1797,11 +1874,11 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="9">
@@ -1822,9 +1899,9 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="8">
         <v>16</v>
       </c>
@@ -1843,11 +1920,11 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="46" t="s">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="49" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="18">
@@ -1868,9 +1945,9 @@
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="19">
         <v>18</v>
       </c>
@@ -1889,11 +1966,11 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="11">
@@ -1914,9 +1991,9 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49"/>
-      <c r="B21" s="52"/>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="12">
         <v>20</v>
       </c>
@@ -1935,9 +2012,9 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="53"/>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="11">
         <v>21</v>
       </c>
@@ -1956,11 +2033,11 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="15">
@@ -1981,9 +2058,9 @@
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32"/>
-      <c r="B24" s="34"/>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="16">
         <v>23</v>
       </c>
@@ -2002,7 +2079,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14">
@@ -2011,15 +2088,15 @@
       <c r="D25" s="14">
         <v>8</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14">
@@ -2028,15 +2105,15 @@
       <c r="D26" s="14">
         <v>9</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14">
@@ -2045,15 +2122,15 @@
       <c r="D27" s="14">
         <v>10</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14">
@@ -2062,19 +2139,19 @@
       <c r="D28" s="14">
         <v>11</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="31" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="6">
@@ -2093,9 +2170,9 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="7">
         <v>29</v>
       </c>
@@ -2114,9 +2191,9 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="6">
         <v>30</v>
       </c>
@@ -2135,9 +2212,9 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="7">
         <v>31</v>
       </c>
@@ -2154,9 +2231,9 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
@@ -2205,57 +2282,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="2.7265625" customWidth="1"/>
-    <col min="10" max="10" width="2.1796875" customWidth="1"/>
-    <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="10" width="2" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.7265625" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="2" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.26953125" customWidth="1"/>
-    <col min="18" max="18" width="7.26953125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="7.26953125" customWidth="1"/>
+    <col min="16" max="17" width="7.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
       <c r="I1" s="24"/>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="57"/>
-      <c r="N1" s="58" t="s">
+      <c r="L1" s="60"/>
+      <c r="N1" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="58"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="O1" s="61"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="24"/>
       <c r="K2" s="21" t="s">
         <v>21</v>
@@ -2271,7 +2347,7 @@
       </c>
       <c r="Q2" s="20"/>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -2297,101 +2373,101 @@
         <v>8</v>
       </c>
       <c r="I3" s="24"/>
-      <c r="K3" s="21">
-        <v>1</v>
+      <c r="K3" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="21">
-        <v>1</v>
+      <c r="N3" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="Q3" s="20"/>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="55" t="s">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="57" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="24"/>
-      <c r="K4" s="21">
-        <v>2</v>
+      <c r="K4" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="L4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="21">
-        <v>2</v>
+      <c r="N4" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>11</v>
       </c>
       <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="24"/>
-      <c r="K5" s="21">
-        <v>3</v>
+      <c r="K5" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="L5" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="21">
-        <v>3</v>
+      <c r="N5" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>64</v>
       </c>
       <c r="Q5" s="20"/>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="24"/>
-      <c r="K6" s="21">
-        <v>4</v>
+      <c r="K6" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="L6" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="21">
-        <v>4</v>
+      <c r="N6" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>65</v>
       </c>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>9</v>
       </c>
@@ -2417,121 +2493,121 @@
         <v>16</v>
       </c>
       <c r="I7" s="24"/>
-      <c r="K7" s="21">
-        <v>5</v>
+      <c r="K7" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="L7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="21">
-        <v>5</v>
+      <c r="N7" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>54</v>
       </c>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="55" t="s">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="55" t="s">
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="56" t="s">
         <v>69</v>
       </c>
       <c r="I8" s="24"/>
-      <c r="K8" s="21">
-        <v>6</v>
+      <c r="K8" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="L8" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="21">
-        <v>6</v>
+      <c r="N8" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="O8" s="21" t="s">
         <v>66</v>
       </c>
       <c r="Q8" s="20"/>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="24"/>
-      <c r="K9" s="21">
-        <v>7</v>
+      <c r="K9" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="L9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="21">
-        <v>7</v>
+      <c r="N9" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="O9" s="21" t="s">
         <v>1</v>
       </c>
       <c r="Q9" s="20"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="24"/>
-      <c r="K10" s="21">
-        <v>8</v>
+      <c r="K10" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="21">
-        <v>8</v>
+      <c r="N10" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="O10" s="21" t="s">
         <v>2</v>
       </c>
       <c r="Q10" s="20"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="24"/>
-      <c r="K11" s="21">
-        <v>9</v>
+      <c r="K11" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="21">
-        <v>9</v>
+      <c r="N11" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="O11" s="21" t="s">
         <v>18</v>
       </c>
       <c r="Q11" s="20"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>1</v>
       </c>
@@ -2557,83 +2633,83 @@
         <v>8</v>
       </c>
       <c r="I12" s="24"/>
-      <c r="K12" s="21">
-        <v>10</v>
+      <c r="K12" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="L12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="21">
-        <v>10</v>
+      <c r="N12" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="O12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="20"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="55" t="s">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="67" t="s">
+      <c r="G13" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="66"/>
+      <c r="H13" s="59"/>
       <c r="I13" s="24"/>
-      <c r="K13" s="21">
-        <v>11</v>
+      <c r="K13" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="L13" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N13" s="21">
-        <v>11</v>
+      <c r="N13" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="O13" s="21" t="s">
         <v>67</v>
       </c>
       <c r="Q13" s="20"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="66"/>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="59"/>
       <c r="I14" s="24"/>
-      <c r="K14" s="21">
-        <v>12</v>
+      <c r="K14" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="L14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N14" s="21">
-        <v>12</v>
+      <c r="N14" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>3</v>
       </c>
       <c r="Q14" s="20"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2643,89 +2719,89 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="24"/>
-      <c r="K15" s="21">
-        <v>13</v>
+      <c r="K15" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="L15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="21">
-        <v>13</v>
+      <c r="N15" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="O15" s="21" t="s">
         <v>4</v>
       </c>
       <c r="Q15" s="20"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="24"/>
-      <c r="K16" s="21">
-        <v>14</v>
+      <c r="K16" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="21">
-        <v>14</v>
+      <c r="N16" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="O16" s="21" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="20"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
       <c r="I17" s="24"/>
-      <c r="K17" s="21">
-        <v>15</v>
+      <c r="K17" s="21" t="s">
+        <v>110</v>
       </c>
       <c r="L17" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N17" s="21">
-        <v>15</v>
+      <c r="N17" s="21" t="s">
+        <v>110</v>
       </c>
       <c r="O17" s="21" t="s">
         <v>49</v>
       </c>
       <c r="Q17" s="20"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+    <row r="18" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
       <c r="I18" s="24"/>
-      <c r="K18" s="21">
-        <v>16</v>
+      <c r="K18" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="L18" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="N18" s="21">
-        <v>16</v>
-      </c>
-      <c r="O18" s="21" t="s">
+      <c r="N18" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="O18" s="29" t="s">
         <v>50</v>
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>1</v>
       </c>
@@ -2751,71 +2827,71 @@
         <v>8</v>
       </c>
       <c r="I19" s="24"/>
-      <c r="N19" s="21">
+      <c r="N19" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="O19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="62" t="s">
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="63" t="s">
+      <c r="C20" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="64" t="s">
+      <c r="G20" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="66"/>
+      <c r="H20" s="59"/>
       <c r="I20" s="24"/>
-      <c r="N20" s="21">
-        <v>18</v>
+      <c r="N20" s="21" t="s">
+        <v>113</v>
       </c>
       <c r="O20" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="66"/>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="59"/>
       <c r="I21" s="24"/>
-      <c r="N21" s="21">
-        <v>19</v>
+      <c r="N21" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="O21" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="24"/>
-      <c r="N22" s="21">
-        <v>20</v>
+      <c r="N22" s="21" t="s">
+        <v>115</v>
       </c>
       <c r="O22" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>9</v>
       </c>
@@ -2841,79 +2917,79 @@
         <v>16</v>
       </c>
       <c r="I23" s="24"/>
-      <c r="N23" s="21">
-        <v>21</v>
+      <c r="N23" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="O23" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="66"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="65" t="s">
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="65" t="s">
+      <c r="H24" s="67" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="24"/>
-      <c r="N24" s="21">
-        <v>22</v>
+      <c r="N24" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="O24" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="66"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
       <c r="I25" s="24"/>
-      <c r="N25" s="21">
-        <v>23</v>
+      <c r="N25" s="28" t="s">
+        <v>118</v>
       </c>
       <c r="O25" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="24"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="21">
-        <v>24</v>
+      <c r="N26" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="O26" s="21"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="56" t="s">
+    <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25"/>
       <c r="K27" s="1"/>
@@ -2922,7 +2998,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>1</v>
       </c>
@@ -2948,113 +3024,115 @@
         <v>8</v>
       </c>
       <c r="I28" s="24"/>
-      <c r="K28" s="59" t="s">
+      <c r="K28" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="69" t="s">
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="70" t="s">
+      <c r="B29" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="71" t="s">
+      <c r="C29" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="72" t="s">
+      <c r="D29" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="75" t="s">
+      <c r="F29" s="59"/>
+      <c r="G29" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="75" t="s">
+      <c r="H29" s="65" t="s">
         <v>85</v>
       </c>
       <c r="I29" s="24"/>
       <c r="K29" s="10">
         <v>1</v>
       </c>
-      <c r="L29" s="60" t="s">
+      <c r="L29" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="69"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
       <c r="I30" s="24"/>
       <c r="K30" s="3">
         <v>2</v>
       </c>
-      <c r="L30" s="61" t="s">
+      <c r="L30" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
-    </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="24"/>
       <c r="K31" s="10">
         <v>3</v>
       </c>
-      <c r="L31" s="60" t="s">
+      <c r="L31" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="60"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="24"/>
       <c r="K32" s="3">
         <v>4</v>
       </c>
-      <c r="L32" s="61" t="s">
+      <c r="L32" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="61"/>
-    </row>
-    <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+    </row>
+    <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I33" s="24"/>
       <c r="K33" s="10">
         <v>5</v>
       </c>
-      <c r="L33" s="60" t="s">
+      <c r="L33" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-    </row>
-    <row r="34" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I34" s="24"/>
       <c r="K34" s="3">
         <v>6</v>
       </c>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
+      <c r="L34" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="63">

</xml_diff>

<commit_message>
Reformatted inputs to match port size
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527ACED8-E34E-4F9C-9086-BF72AFC8BF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0505AC16-F23C-4325-BEB6-D7D87F0A925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="126">
   <si>
     <t>Input</t>
   </si>
@@ -405,6 +405,22 @@
   </si>
   <si>
     <t>Bottom</t>
+  </si>
+  <si>
+    <t>Paul
+IEM</t>
+  </si>
+  <si>
+    <t>John
+IEM</t>
+  </si>
+  <si>
+    <t>Kenzi
+IEM</t>
+  </si>
+  <si>
+    <t>Talk
+Back</t>
   </si>
 </sst>
 </file>
@@ -908,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -953,170 +969,137 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1124,6 +1107,42 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1298,9 +1317,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1338,7 +1357,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1444,7 +1463,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1586,7 +1605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1892,13 +1911,13 @@
       <c r="D12" s="26">
         <v>11</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
@@ -1909,13 +1928,13 @@
       <c r="D13" s="27">
         <v>12</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
@@ -1960,10 +1979,10 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="43" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="9">
@@ -1985,8 +2004,8 @@
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="8">
         <v>16</v>
       </c>
@@ -2006,10 +2025,10 @@
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="51" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="18">
@@ -2031,8 +2050,8 @@
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="19">
         <v>18</v>
       </c>
@@ -2052,10 +2071,10 @@
       <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="55" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="11">
@@ -2077,8 +2096,8 @@
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="12">
         <v>20</v>
       </c>
@@ -2098,8 +2117,8 @@
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="11">
         <v>21</v>
       </c>
@@ -2119,10 +2138,10 @@
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="15">
@@ -2144,8 +2163,8 @@
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="55"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="16">
         <v>23</v>
       </c>
@@ -2173,13 +2192,13 @@
       <c r="D25" s="14">
         <v>8</v>
       </c>
-      <c r="E25" s="51" t="s">
+      <c r="E25" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
@@ -2190,13 +2209,13 @@
       <c r="D26" s="14">
         <v>9</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
@@ -2207,13 +2226,13 @@
       <c r="D27" s="14">
         <v>10</v>
       </c>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
@@ -2224,19 +2243,19 @@
       <c r="D28" s="14">
         <v>11</v>
       </c>
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="6">
@@ -2256,8 +2275,8 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="7">
         <v>29</v>
       </c>
@@ -2277,8 +2296,8 @@
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="6">
         <v>30</v>
       </c>
@@ -2298,8 +2317,8 @@
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="7">
         <v>31</v>
       </c>
@@ -2317,8 +2336,8 @@
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
@@ -2337,6 +2356,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B15"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E12:I12"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="E26:I26"/>
@@ -2345,17 +2375,6 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="E28:I28"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="B2:B15"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2368,7 +2387,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O26"/>
+      <selection activeCell="B29" sqref="B29:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,37 +2405,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="24"/>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="69"/>
-      <c r="N1" s="70" t="s">
+      <c r="L1" s="62"/>
+      <c r="N1" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="70"/>
+      <c r="O1" s="63"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="24"/>
       <c r="K2" s="21" t="s">
         <v>21</v>
@@ -2473,28 +2492,28 @@
       <c r="Q3" s="20"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="59" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="24"/>
@@ -2513,14 +2532,14 @@
       <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="24"/>
       <c r="K5" s="21" t="s">
         <v>98</v>
@@ -2593,22 +2612,22 @@
       <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="58" t="s">
         <v>69</v>
       </c>
       <c r="I8" s="24"/>
@@ -2627,14 +2646,14 @@
       <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="24"/>
       <c r="K9" s="21" t="s">
         <v>102</v>
@@ -2667,16 +2686,16 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="24"/>
       <c r="K11" s="21" t="s">
         <v>104</v>
@@ -2733,28 +2752,28 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="61" t="s">
+      <c r="F13" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="61" t="s">
+      <c r="G13" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="56"/>
+      <c r="H13" s="61"/>
       <c r="I13" s="24"/>
       <c r="K13" s="21" t="s">
         <v>106</v>
@@ -2771,14 +2790,14 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="56"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="24"/>
       <c r="K14" s="21" t="s">
         <v>107</v>
@@ -2835,16 +2854,16 @@
       <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
       <c r="I17" s="24"/>
       <c r="K17" s="21" t="s">
         <v>110</v>
@@ -2861,16 +2880,16 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
       <c r="I18" s="24"/>
       <c r="K18" s="21" t="s">
         <v>111</v>
@@ -2920,28 +2939,28 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="56"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="24"/>
       <c r="N20" s="21" t="s">
         <v>113</v>
@@ -2951,14 +2970,14 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="56"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="61"/>
       <c r="I21" s="24"/>
       <c r="N21" s="28" t="s">
         <v>114</v>
@@ -3010,22 +3029,22 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="60" t="s">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="60" t="s">
+      <c r="G24" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="60" t="s">
+      <c r="H24" s="69" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="24"/>
@@ -3037,14 +3056,14 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
       <c r="I25" s="24"/>
       <c r="N25" s="28" t="s">
         <v>118</v>
@@ -3065,16 +3084,16 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25"/>
       <c r="K27" s="1"/>
@@ -3109,118 +3128,165 @@
         <v>8</v>
       </c>
       <c r="I28" s="24"/>
-      <c r="K28" s="71" t="s">
+      <c r="K28" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="71"/>
-      <c r="M28" s="71"/>
-      <c r="N28" s="71"/>
-      <c r="O28" s="71"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D29" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="65" t="s">
+      <c r="F29" s="61"/>
+      <c r="G29" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="65" t="s">
+      <c r="H29" s="67" t="s">
         <v>85</v>
       </c>
       <c r="I29" s="24"/>
       <c r="K29" s="10">
         <v>1</v>
       </c>
-      <c r="L29" s="67" t="s">
+      <c r="L29" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="M29" s="67"/>
-      <c r="N29" s="67"/>
-      <c r="O29" s="67"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
       <c r="I30" s="24"/>
       <c r="K30" s="3">
         <v>2</v>
       </c>
-      <c r="L30" s="68" t="s">
+      <c r="L30" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="68"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="24"/>
       <c r="K31" s="10">
         <v>3</v>
       </c>
-      <c r="L31" s="67" t="s">
+      <c r="L31" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="24"/>
       <c r="K32" s="3">
         <v>4</v>
       </c>
-      <c r="L32" s="68" t="s">
+      <c r="L32" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="66"/>
     </row>
     <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I33" s="24"/>
       <c r="K33" s="10">
         <v>5</v>
       </c>
-      <c r="L33" s="67" t="s">
+      <c r="L33" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="M33" s="67"/>
-      <c r="N33" s="67"/>
-      <c r="O33" s="67"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
     </row>
     <row r="34" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I34" s="24"/>
       <c r="K34" s="3">
         <v>6</v>
       </c>
-      <c r="L34" s="68" t="s">
+      <c r="L34" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L30:O30"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A11:H11"/>
@@ -3237,53 +3303,6 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3297,228 +3316,282 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728856F4-176B-4634-AD3E-524669928A0A}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="21" width="14.5703125" customWidth="1"/>
+    <col min="1" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="22" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="86" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="J1" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-    </row>
-    <row r="2" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75">
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+    </row>
+    <row r="2" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="75">
+      <c r="B2" s="31">
         <v>2</v>
       </c>
-      <c r="C2" s="75">
+      <c r="C2" s="31">
         <v>3</v>
       </c>
-      <c r="D2" s="75">
+      <c r="D2" s="31">
         <v>4</v>
       </c>
-      <c r="E2" s="75">
+      <c r="E2" s="31">
         <v>5</v>
       </c>
-      <c r="F2" s="75">
+      <c r="F2" s="31">
         <v>6</v>
       </c>
-      <c r="G2" s="75">
+      <c r="G2" s="31">
         <v>7</v>
       </c>
-      <c r="H2" s="75">
+      <c r="H2" s="31">
         <v>8</v>
       </c>
-      <c r="I2" s="75">
+      <c r="J2" s="31">
         <v>9</v>
       </c>
-      <c r="J2" s="75">
+      <c r="K2" s="31">
         <v>10</v>
       </c>
-      <c r="K2" s="75">
+      <c r="L2" s="31">
         <v>11</v>
       </c>
-      <c r="L2" s="75">
+      <c r="M2" s="31">
         <v>12</v>
       </c>
-      <c r="M2" s="75">
+      <c r="N2" s="31">
         <v>13</v>
       </c>
-      <c r="N2" s="75">
+      <c r="O2" s="31">
         <v>14</v>
       </c>
-      <c r="O2" s="75">
+      <c r="P2" s="31">
         <v>15</v>
       </c>
-      <c r="P2" s="75">
+      <c r="Q2" s="31">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+    <row r="3" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="81" t="s">
+      <c r="H3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="J3" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="K3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="L3" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="M3" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="N3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="84" t="s">
+      <c r="O3" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="85" t="s">
+      <c r="P3" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="84" t="s">
+      <c r="Q3" s="85" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-    </row>
-    <row r="5" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
+    <row r="4" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-    </row>
-    <row r="6" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75">
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="J5" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+    </row>
+    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>17</v>
       </c>
-      <c r="B6" s="75">
+      <c r="B6" s="31">
         <v>18</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="31">
         <v>19</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="31">
         <v>20</v>
       </c>
-      <c r="E6" s="75">
+      <c r="E6" s="31">
         <v>21</v>
       </c>
-      <c r="F6" s="75">
+      <c r="F6" s="31">
         <v>22</v>
       </c>
-      <c r="G6" s="75">
+      <c r="G6" s="31">
         <v>23</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="31">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
+      <c r="J6" s="31">
+        <v>25</v>
+      </c>
+      <c r="K6" s="31">
+        <v>26</v>
+      </c>
+      <c r="L6" s="31">
+        <v>27</v>
+      </c>
+      <c r="M6" s="31">
+        <v>28</v>
+      </c>
+      <c r="N6" s="31">
+        <v>29</v>
+      </c>
+      <c r="O6" s="31">
+        <v>30</v>
+      </c>
+      <c r="P6" s="31">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="77" t="s">
+      <c r="F7" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="G7" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="73"/>
-    </row>
-    <row r="8" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="74"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-    </row>
-    <row r="9" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="M7" s="79" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="86" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="J1:Q1"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="J5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated metadata on input list
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0505AC16-F23C-4325-BEB6-D7D87F0A925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED86617A-5E99-44A5-999A-F55914318321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="130">
   <si>
     <t>Input</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Internal</t>
   </si>
   <si>
-    <t>Clip</t>
-  </si>
-  <si>
     <t>Shure SM137</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>Shure 55SH</t>
-  </si>
-  <si>
-    <t>Hang Stand</t>
   </si>
   <si>
     <t>Sennheiser E609</t>
@@ -421,6 +415,24 @@
   <si>
     <t>Talk
 Back</t>
+  </si>
+  <si>
+    <t>Amp Mic Stand</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Drum Clamp</t>
+  </si>
+  <si>
+    <t>Bongo Stand</t>
+  </si>
+  <si>
+    <t>Hanging Mic Stand</t>
+  </si>
+  <si>
+    <t>Boom Mic Stand</t>
   </si>
 </sst>
 </file>
@@ -748,7 +760,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -832,54 +844,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -924,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -965,14 +929,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -982,166 +992,82 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1317,9 +1243,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1357,7 +1283,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1463,7 +1389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1605,7 +1531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1615,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,24 +1553,24 @@
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" customWidth="1"/>
     <col min="10" max="22" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>0</v>
@@ -1663,11 +1589,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>31</v>
+      <c r="A2" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1686,12 +1612,12 @@
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="5">
         <v>2</v>
       </c>
@@ -1705,14 +1631,14 @@
         <v>26</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="4">
         <v>3</v>
       </c>
@@ -1723,21 +1649,21 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
@@ -1751,18 +1677,18 @@
         <v>27</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="4">
         <v>5</v>
       </c>
@@ -1776,18 +1702,18 @@
         <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="5">
         <v>6</v>
       </c>
@@ -1801,18 +1727,18 @@
         <v>27</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
@@ -1826,18 +1752,18 @@
         <v>27</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
@@ -1845,24 +1771,24 @@
         <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="4">
         <v>9</v>
       </c>
@@ -1870,75 +1796,75 @@
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="E11" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="4">
         <v>11</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="49"/>
+      <c r="E12" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="5">
         <v>12</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="5">
         <v>12</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="46"/>
+      <c r="E13" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="4">
         <v>13</v>
       </c>
@@ -1946,20 +1872,20 @@
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="5">
         <v>14</v>
       </c>
@@ -1973,17 +1899,17 @@
         <v>26</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>41</v>
+      <c r="A16" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>40</v>
       </c>
       <c r="C16" s="9">
         <v>15</v>
@@ -1992,20 +1918,20 @@
         <v>15</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="8">
         <v>16</v>
       </c>
@@ -2013,23 +1939,23 @@
         <v>16</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="51" t="s">
-        <v>44</v>
+      <c r="A18" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>43</v>
       </c>
       <c r="C18" s="18">
         <v>17</v>
@@ -2038,20 +1964,20 @@
         <v>1</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="19">
         <v>18</v>
       </c>
@@ -2059,23 +1985,23 @@
         <v>2</v>
       </c>
       <c r="E19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>68</v>
-      </c>
       <c r="G19" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>37</v>
+      <c r="A20" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="72" t="s">
+        <v>36</v>
       </c>
       <c r="C20" s="11">
         <v>19</v>
@@ -2087,17 +2013,17 @@
         <v>18</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="12">
         <v>20</v>
       </c>
@@ -2108,17 +2034,17 @@
         <v>19</v>
       </c>
       <c r="F21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
-      <c r="B22" s="57"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="11">
         <v>21</v>
       </c>
@@ -2126,23 +2052,23 @@
         <v>5</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>43</v>
+      <c r="A23" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>42</v>
       </c>
       <c r="C23" s="15">
         <v>22</v>
@@ -2154,17 +2080,17 @@
         <v>1</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="38"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="16">
         <v>23</v>
       </c>
@@ -2175,10 +2101,10 @@
         <v>2</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -2192,13 +2118,13 @@
       <c r="D25" s="14">
         <v>8</v>
       </c>
-      <c r="E25" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
+      <c r="E25" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
@@ -2209,13 +2135,13 @@
       <c r="D26" s="14">
         <v>9</v>
       </c>
-      <c r="E26" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
+      <c r="E26" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
@@ -2226,13 +2152,13 @@
       <c r="D27" s="14">
         <v>10</v>
       </c>
-      <c r="E27" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
+      <c r="E27" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
@@ -2243,20 +2169,20 @@
       <c r="D28" s="14">
         <v>11</v>
       </c>
-      <c r="E28" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
+      <c r="E28" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>38</v>
+      <c r="A29" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="6">
         <v>28</v>
@@ -2265,18 +2191,20 @@
         <v>12</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="G29" s="6" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="7">
         <v>29</v>
       </c>
@@ -2284,20 +2212,20 @@
         <v>13</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="6">
         <v>30</v>
       </c>
@@ -2308,17 +2236,17 @@
         <v>3</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="7">
         <v>31</v>
       </c>
@@ -2328,16 +2256,18 @@
       <c r="E32" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="G32" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
@@ -2345,28 +2275,19 @@
         <v>16</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="G33" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="B2:B15"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E12:I12"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="E26:I26"/>
@@ -2375,6 +2296,17 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="E28:I28"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B15"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2405,49 +2337,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="A1" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
       <c r="I1" s="24"/>
       <c r="K1" s="62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L1" s="62"/>
       <c r="N1" s="63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O1" s="63"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="24"/>
       <c r="K2" s="21" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="20"/>
     </row>
@@ -2478,13 +2410,13 @@
       </c>
       <c r="I3" s="24"/>
       <c r="K3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>10</v>
@@ -2492,39 +2424,39 @@
       <c r="Q3" s="20"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>65</v>
+      <c r="H4" s="50" t="s">
+        <v>63</v>
       </c>
       <c r="I4" s="24"/>
       <c r="K4" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L4" s="21" t="s">
         <v>11</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>11</v>
@@ -2532,42 +2464,42 @@
       <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="24"/>
       <c r="K5" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q5" s="20"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="24"/>
       <c r="K6" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q6" s="20"/>
     </row>
@@ -2598,71 +2530,71 @@
       </c>
       <c r="I7" s="24"/>
       <c r="K7" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="59" t="s">
+      <c r="A8" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>69</v>
+      <c r="G8" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>67</v>
       </c>
       <c r="I8" s="24"/>
       <c r="K8" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="24"/>
       <c r="K9" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L9" s="21" t="s">
         <v>1</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O9" s="21" t="s">
         <v>1</v>
@@ -2672,13 +2604,13 @@
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="24"/>
       <c r="K10" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>2</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O10" s="21" t="s">
         <v>2</v>
@@ -2686,25 +2618,25 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="24"/>
       <c r="K11" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>18</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O11" s="21" t="s">
         <v>18</v>
@@ -2738,13 +2670,13 @@
       </c>
       <c r="I12" s="24"/>
       <c r="K12" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O12" s="21" t="s">
         <v>19</v>
@@ -2752,61 +2684,61 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="61"/>
+      <c r="G13" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="49"/>
       <c r="I13" s="24"/>
       <c r="K13" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="61"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="24"/>
       <c r="K14" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L14" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O14" s="21" t="s">
         <v>3</v>
@@ -2824,13 +2756,13 @@
       <c r="H15" s="1"/>
       <c r="I15" s="24"/>
       <c r="K15" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L15" s="21" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O15" s="21" t="s">
         <v>4</v>
@@ -2840,13 +2772,13 @@
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="24"/>
       <c r="K16" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>5</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O16" s="21" t="s">
         <v>5</v>
@@ -2854,54 +2786,54 @@
       <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
+      <c r="A17" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
       <c r="I17" s="24"/>
       <c r="K17" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
       <c r="I18" s="24"/>
       <c r="K18" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L18" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="N18" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="O18" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Q18" s="20"/>
     </row>
@@ -2931,56 +2863,56 @@
         <v>8</v>
       </c>
       <c r="I19" s="24"/>
-      <c r="N19" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="O19" s="28" t="s">
+      <c r="N19" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="O19" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="71" t="s">
+      <c r="A20" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="74" t="s">
+      <c r="E20" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="74" t="s">
+      <c r="G20" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="61"/>
+      <c r="H20" s="49"/>
       <c r="I20" s="24"/>
       <c r="N20" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O20" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="61"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="49"/>
       <c r="I21" s="24"/>
-      <c r="N21" s="28" t="s">
-        <v>114</v>
+      <c r="N21" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="O21" s="21" t="s">
         <v>13</v>
@@ -2989,7 +2921,7 @@
     <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="24"/>
       <c r="N22" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O22" s="21" t="s">
         <v>14</v>
@@ -3021,55 +2953,55 @@
         <v>16</v>
       </c>
       <c r="I23" s="24"/>
-      <c r="N23" s="28" t="s">
-        <v>116</v>
+      <c r="N23" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="O23" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="69" t="s">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="69" t="s">
+      <c r="E24" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="69" t="s">
+      <c r="G24" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="69" t="s">
+      <c r="H24" s="53" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="24"/>
       <c r="N24" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O24" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="24"/>
-      <c r="N25" s="28" t="s">
-        <v>118</v>
+      <c r="N25" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3078,22 +3010,22 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O26" s="21"/>
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25"/>
       <c r="K27" s="1"/>
@@ -3137,122 +3069,143 @@
       <c r="O28" s="64"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="69" t="s">
+      <c r="E29" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="67" t="s">
+      <c r="F29" s="49"/>
+      <c r="G29" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="67" t="s">
-        <v>85</v>
+      <c r="H29" s="58" t="s">
+        <v>83</v>
       </c>
       <c r="I29" s="24"/>
       <c r="K29" s="10">
         <v>1</v>
       </c>
-      <c r="L29" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="65"/>
+      <c r="L29" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
       <c r="I30" s="24"/>
       <c r="K30" s="3">
         <v>2</v>
       </c>
-      <c r="L30" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="M30" s="66"/>
-      <c r="N30" s="66"/>
-      <c r="O30" s="66"/>
+      <c r="L30" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="24"/>
       <c r="K31" s="10">
         <v>3</v>
       </c>
-      <c r="L31" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="M31" s="65"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
+      <c r="L31" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="24"/>
       <c r="K32" s="3">
         <v>4</v>
       </c>
-      <c r="L32" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="M32" s="66"/>
-      <c r="N32" s="66"/>
-      <c r="O32" s="66"/>
+      <c r="L32" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
     </row>
     <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I33" s="24"/>
       <c r="K33" s="10">
         <v>5</v>
       </c>
-      <c r="L33" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="M33" s="65"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
+      <c r="L33" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
     </row>
     <row r="34" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I34" s="24"/>
       <c r="K34" s="3">
         <v>6</v>
       </c>
-      <c r="L34" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="M34" s="66"/>
-      <c r="N34" s="66"/>
-      <c r="O34" s="66"/>
+      <c r="L34" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
@@ -3269,40 +3222,19 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3318,7 +3250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728856F4-176B-4634-AD3E-524669928A0A}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -3329,260 +3261,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="J1" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+    </row>
+    <row r="2" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29">
+        <v>3</v>
+      </c>
+      <c r="D2" s="29">
+        <v>4</v>
+      </c>
+      <c r="E2" s="29">
+        <v>5</v>
+      </c>
+      <c r="F2" s="29">
+        <v>6</v>
+      </c>
+      <c r="G2" s="29">
+        <v>7</v>
+      </c>
+      <c r="H2" s="29">
+        <v>8</v>
+      </c>
+      <c r="J2" s="29">
+        <v>9</v>
+      </c>
+      <c r="K2" s="29">
+        <v>10</v>
+      </c>
+      <c r="L2" s="29">
+        <v>11</v>
+      </c>
+      <c r="M2" s="29">
+        <v>12</v>
+      </c>
+      <c r="N2" s="29">
+        <v>13</v>
+      </c>
+      <c r="O2" s="29">
+        <v>14</v>
+      </c>
+      <c r="P2" s="29">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="J5" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+    </row>
+    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>17</v>
+      </c>
+      <c r="B6" s="29">
+        <v>18</v>
+      </c>
+      <c r="C6" s="29">
+        <v>19</v>
+      </c>
+      <c r="D6" s="29">
+        <v>20</v>
+      </c>
+      <c r="E6" s="29">
+        <v>21</v>
+      </c>
+      <c r="F6" s="29">
+        <v>22</v>
+      </c>
+      <c r="G6" s="29">
+        <v>23</v>
+      </c>
+      <c r="H6" s="29">
+        <v>24</v>
+      </c>
+      <c r="J6" s="29">
+        <v>25</v>
+      </c>
+      <c r="K6" s="29">
+        <v>26</v>
+      </c>
+      <c r="L6" s="29">
+        <v>27</v>
+      </c>
+      <c r="M6" s="29">
+        <v>28</v>
+      </c>
+      <c r="N6" s="29">
+        <v>29</v>
+      </c>
+      <c r="O6" s="29">
+        <v>30</v>
+      </c>
+      <c r="P6" s="29">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="J1" s="75" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-    </row>
-    <row r="2" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
-        <v>1</v>
-      </c>
-      <c r="B2" s="31">
-        <v>2</v>
-      </c>
-      <c r="C2" s="31">
-        <v>3</v>
-      </c>
-      <c r="D2" s="31">
-        <v>4</v>
-      </c>
-      <c r="E2" s="31">
-        <v>5</v>
-      </c>
-      <c r="F2" s="31">
-        <v>6</v>
-      </c>
-      <c r="G2" s="31">
-        <v>7</v>
-      </c>
-      <c r="H2" s="31">
-        <v>8</v>
-      </c>
-      <c r="J2" s="31">
-        <v>9</v>
-      </c>
-      <c r="K2" s="31">
-        <v>10</v>
-      </c>
-      <c r="L2" s="31">
-        <v>11</v>
-      </c>
-      <c r="M2" s="31">
-        <v>12</v>
-      </c>
-      <c r="N2" s="31">
-        <v>13</v>
-      </c>
-      <c r="O2" s="31">
-        <v>14</v>
-      </c>
-      <c r="P2" s="31">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="87" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="84" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" s="85" t="s">
-        <v>5</v>
-      </c>
-      <c r="P3" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="85" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="L7" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="J5" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-    </row>
-    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>17</v>
-      </c>
-      <c r="B6" s="31">
-        <v>18</v>
-      </c>
-      <c r="C6" s="31">
-        <v>19</v>
-      </c>
-      <c r="D6" s="31">
-        <v>20</v>
-      </c>
-      <c r="E6" s="31">
-        <v>21</v>
-      </c>
-      <c r="F6" s="31">
-        <v>22</v>
-      </c>
-      <c r="G6" s="31">
-        <v>23</v>
-      </c>
-      <c r="H6" s="31">
-        <v>24</v>
-      </c>
-      <c r="J6" s="31">
-        <v>25</v>
-      </c>
-      <c r="K6" s="31">
-        <v>26</v>
-      </c>
-      <c r="L6" s="31">
-        <v>27</v>
-      </c>
-      <c r="M6" s="31">
-        <v>28</v>
-      </c>
-      <c r="N6" s="31">
-        <v>29</v>
-      </c>
-      <c r="O6" s="31">
-        <v>30</v>
-      </c>
-      <c r="P6" s="31">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="31">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="L7" s="85" t="s">
-        <v>124</v>
-      </c>
-      <c r="M7" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="N7" s="84" t="s">
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="86" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="8" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved to name ranges
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA336841-BBD2-401F-839F-ECF58ACA7418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143597C9-C6A0-4099-9DFF-DAE32D522C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -16,6 +16,18 @@
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Snake + PA" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_48v">'Input + Equipment'!$H$4:$H$35</definedName>
+    <definedName name="Channel">'Input + Equipment'!$C$4:$C$35</definedName>
+    <definedName name="Input">'Input + Equipment'!$E$4:$E$35</definedName>
+    <definedName name="InputEquipmnetExportRange">'Input + Equipment'!$A$3:$I$35</definedName>
+    <definedName name="Mic_DI">'Input + Equipment'!$F$4:$F$35</definedName>
+    <definedName name="Musician">'Input + Equipment'!$A$4:$A$35</definedName>
+    <definedName name="Notes">'Input + Equipment'!$I$4:$I$35</definedName>
+    <definedName name="Position">'Input + Equipment'!$B$4:$B$35</definedName>
+    <definedName name="Snake">'Input + Equipment'!$D$4:$D$35</definedName>
+    <definedName name="Stand">'Input + Equipment'!$G$4:$G$35</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -777,37 +789,31 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,9 +839,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -854,26 +857,92 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -887,68 +956,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1345,7 +1357,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A3" sqref="A3:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,32 +1375,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="e" vm="1">
+      <c r="A1" s="33" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="37" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1420,10 +1432,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="42" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="16">
@@ -1447,8 +1459,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="46"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -1470,8 +1482,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="16">
         <v>3</v>
       </c>
@@ -1491,8 +1503,8 @@
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="46"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -1516,8 +1528,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="46"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="16">
         <v>5</v>
       </c>
@@ -1541,8 +1553,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="46"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -1566,8 +1578,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="46"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="16">
         <v>7</v>
       </c>
@@ -1591,8 +1603,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -1616,8 +1628,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="16">
         <v>9</v>
       </c>
@@ -1641,8 +1653,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="1">
         <v>10</v>
       </c>
@@ -1674,13 +1686,13 @@
       <c r="D14" s="5">
         <v>11</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
@@ -1691,13 +1703,13 @@
       <c r="D15" s="5">
         <v>12</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
@@ -1708,13 +1720,13 @@
       <c r="D16" s="5">
         <v>13</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
@@ -1725,19 +1737,19 @@
       <c r="D17" s="5">
         <v>14</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="3">
@@ -1759,8 +1771,8 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="13">
         <v>16</v>
       </c>
@@ -1780,10 +1792,10 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="51" t="s">
         <v>96</v>
       </c>
       <c r="C20" s="14">
@@ -1807,8 +1819,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="15">
         <v>18</v>
       </c>
@@ -1828,8 +1840,8 @@
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="14">
         <v>19</v>
       </c>
@@ -1849,10 +1861,10 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="54" t="s">
         <v>98</v>
       </c>
       <c r="C23" s="8">
@@ -1876,8 +1888,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="9">
         <v>21</v>
       </c>
@@ -1897,10 +1909,10 @@
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="47" t="s">
         <v>99</v>
       </c>
       <c r="C25" s="20">
@@ -1924,8 +1936,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="6">
         <v>23</v>
       </c>
@@ -1953,13 +1965,13 @@
       <c r="D27" s="5">
         <v>8</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -1970,19 +1982,19 @@
       <c r="D28" s="5">
         <v>9</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
     </row>
     <row r="29" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="29" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="19">
@@ -2006,8 +2018,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="2">
         <v>27</v>
       </c>
@@ -2027,8 +2039,8 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="19">
         <v>28</v>
       </c>
@@ -2048,8 +2060,8 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="2">
         <v>29</v>
       </c>
@@ -2069,8 +2081,8 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
-      <c r="B33" s="54"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="19">
         <v>30</v>
       </c>
@@ -2090,10 +2102,10 @@
       <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="24" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="3">
@@ -2117,8 +2129,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
-      <c r="B35" s="48"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="13">
         <v>32</v>
       </c>
@@ -2141,11 +2153,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="G1:I2"/>
@@ -2157,13 +2171,11 @@
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2188,91 +2200,91 @@
     <col min="14" max="14" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="e" vm="1">
+    <row r="1" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="37" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-    </row>
-    <row r="2" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+    </row>
+    <row r="2" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="12"/>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="12"/>
-      <c r="K4" s="56">
+      <c r="K4" s="75">
         <v>1</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -2300,66 +2312,66 @@
         <v>8</v>
       </c>
       <c r="I5" s="12"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="71" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="K6" s="55">
+      <c r="K6" s="74">
         <v>2</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="68"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="72"/>
       <c r="I7" s="12"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
@@ -2371,16 +2383,16 @@
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="56">
+      <c r="K8" s="75">
         <v>3</v>
       </c>
-      <c r="L8" s="58" t="s">
+      <c r="L8" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
@@ -2408,90 +2420,90 @@
         <v>16</v>
       </c>
       <c r="I9" s="12"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="69" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="69" t="s">
+      <c r="H10" s="67" t="s">
         <v>90</v>
       </c>
       <c r="I10" s="12"/>
-      <c r="K10" s="55">
+      <c r="K10" s="74">
         <v>4</v>
       </c>
-      <c r="L10" s="60" t="s">
+      <c r="L10" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="12"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="78"/>
+      <c r="P11" s="78"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="12"/>
-      <c r="K12" s="56">
+      <c r="K12" s="75">
         <v>5</v>
       </c>
-      <c r="L12" s="61" t="s">
+      <c r="L12" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
       <c r="I13" s="12"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
@@ -2519,55 +2531,55 @@
         <v>8</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="55">
+      <c r="K14" s="74">
         <v>6</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="12"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2585,29 +2597,29 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,39 +2650,39 @@
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="66" t="s">
+      <c r="D22" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="74" t="s">
+      <c r="G22" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="62"/>
+      <c r="H22" s="64"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="62"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="64"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2712,55 +2724,55 @@
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
-      <c r="B26" s="72" t="s">
+      <c r="A26" s="69"/>
+      <c r="B26" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="69" t="s">
+      <c r="G26" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="69" t="s">
+      <c r="H26" s="67" t="s">
         <v>85</v>
       </c>
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2791,39 +2803,39 @@
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="76" t="s">
+      <c r="D31" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="77" t="s">
+      <c r="E31" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="62"/>
-      <c r="G31" s="75" t="s">
+      <c r="F31" s="64"/>
+      <c r="G31" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="75" t="s">
+      <c r="H31" s="59" t="s">
         <v>66</v>
       </c>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2833,34 +2845,32 @@
     <row r="35" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:P5"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="L8:P9"/>
+    <mergeCell ref="L10:P11"/>
+    <mergeCell ref="L12:P13"/>
+    <mergeCell ref="L14:P15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="K1:P2"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
@@ -2877,32 +2887,34 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="L14:P15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:P5"/>
-    <mergeCell ref="L6:P7"/>
-    <mergeCell ref="L8:P9"/>
-    <mergeCell ref="L10:P11"/>
-    <mergeCell ref="L12:P13"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added quotes to range
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D661F5E-DD37-4CD7-8F12-A2A368277128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D76353C-BEA0-4930-885A-F6955219DC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -789,31 +789,37 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -839,6 +845,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -857,34 +866,94 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -892,75 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1375,32 +1375,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="e" vm="1">
+      <c r="A1" s="35" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="35" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1432,10 +1432,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="45" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="16">
@@ -1459,8 +1459,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
@@ -1482,8 +1482,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="16">
         <v>3</v>
       </c>
@@ -1503,8 +1503,8 @@
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -1528,8 +1528,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="16">
         <v>5</v>
       </c>
@@ -1553,8 +1553,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="1">
         <v>6</v>
       </c>
@@ -1578,8 +1578,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="16">
         <v>7</v>
       </c>
@@ -1603,8 +1603,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="1">
         <v>8</v>
       </c>
@@ -1628,8 +1628,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="16">
         <v>9</v>
       </c>
@@ -1653,8 +1653,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="1">
         <v>10</v>
       </c>
@@ -1686,13 +1686,13 @@
       <c r="D14" s="5">
         <v>11</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
@@ -1703,13 +1703,13 @@
       <c r="D15" s="5">
         <v>12</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
@@ -1720,13 +1720,13 @@
       <c r="D16" s="5">
         <v>13</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
@@ -1737,19 +1737,19 @@
       <c r="D17" s="5">
         <v>14</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="3">
@@ -1771,8 +1771,8 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="13">
         <v>16</v>
       </c>
@@ -1792,10 +1792,10 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C20" s="14">
@@ -1819,8 +1819,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="15">
         <v>18</v>
       </c>
@@ -1840,8 +1840,8 @@
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="14">
         <v>19</v>
       </c>
@@ -1861,10 +1861,10 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="33" t="s">
         <v>98</v>
       </c>
       <c r="C23" s="8">
@@ -1888,8 +1888,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="9">
         <v>21</v>
       </c>
@@ -1909,10 +1909,10 @@
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="26" t="s">
         <v>99</v>
       </c>
       <c r="C25" s="20">
@@ -1936,8 +1936,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="48"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="6">
         <v>23</v>
       </c>
@@ -1965,13 +1965,13 @@
       <c r="D27" s="5">
         <v>8</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -1982,19 +1982,19 @@
       <c r="D28" s="5">
         <v>9</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="52" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="19">
@@ -2018,8 +2018,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="30"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="2">
         <v>27</v>
       </c>
@@ -2039,8 +2039,8 @@
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="19">
         <v>28</v>
       </c>
@@ -2060,8 +2060,8 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="2">
         <v>29</v>
       </c>
@@ -2081,8 +2081,8 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="51"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="19">
         <v>30</v>
       </c>
@@ -2102,10 +2102,10 @@
       <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="48" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="3">
@@ -2129,8 +2129,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="13">
         <v>32</v>
       </c>
@@ -2153,13 +2153,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="G1:I2"/>
@@ -2171,11 +2169,13 @@
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="E17:I17"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2201,90 +2201,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="e" vm="1">
+      <c r="A1" s="35" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="35" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
       <c r="I3" s="12"/>
-      <c r="K3" s="74" t="s">
+      <c r="K3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="12"/>
-      <c r="K4" s="75">
+      <c r="K4" s="56">
         <v>1</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -2312,66 +2312,66 @@
         <v>8</v>
       </c>
       <c r="I5" s="12"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="71" t="s">
+      <c r="H6" s="67" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="K6" s="74">
+      <c r="K6" s="55">
         <v>2</v>
       </c>
-      <c r="L6" s="73" t="s">
+      <c r="L6" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="72"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="12"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
@@ -2383,16 +2383,16 @@
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="75">
+      <c r="K8" s="56">
         <v>3</v>
       </c>
-      <c r="L8" s="77" t="s">
+      <c r="L8" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="77"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
@@ -2420,90 +2420,90 @@
         <v>16</v>
       </c>
       <c r="I9" s="12"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="67" t="s">
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="67" t="s">
+      <c r="H10" s="69" t="s">
         <v>90</v>
       </c>
       <c r="I10" s="12"/>
-      <c r="K10" s="74">
+      <c r="K10" s="55">
         <v>4</v>
       </c>
-      <c r="L10" s="78" t="s">
+      <c r="L10" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="78"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
       <c r="I11" s="12"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="12"/>
-      <c r="K12" s="75">
+      <c r="K12" s="56">
         <v>5</v>
       </c>
-      <c r="L12" s="79" t="s">
+      <c r="L12" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="79"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
       <c r="I13" s="12"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
@@ -2531,55 +2531,55 @@
         <v>8</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="74">
+      <c r="K14" s="55">
         <v>6</v>
       </c>
-      <c r="L14" s="73" t="s">
+      <c r="L14" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="59"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="58" t="s">
+      <c r="F15" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="12"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2597,29 +2597,29 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2650,39 +2650,39 @@
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="64"/>
+      <c r="H22" s="62"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="64"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="62"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2724,55 +2724,55 @@
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="65" t="s">
+      <c r="A26" s="70"/>
+      <c r="B26" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="65" t="s">
+      <c r="F26" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="67" t="s">
+      <c r="G26" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="67" t="s">
+      <c r="H26" s="69" t="s">
         <v>85</v>
       </c>
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2803,39 +2803,39 @@
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="63" t="s">
+      <c r="E31" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="64"/>
-      <c r="G31" s="59" t="s">
+      <c r="F31" s="62"/>
+      <c r="G31" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="59" t="s">
+      <c r="H31" s="75" t="s">
         <v>66</v>
       </c>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="58"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2845,32 +2845,34 @@
     <row r="35" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:P5"/>
-    <mergeCell ref="L6:P7"/>
-    <mergeCell ref="L8:P9"/>
-    <mergeCell ref="L10:P11"/>
-    <mergeCell ref="L12:P13"/>
-    <mergeCell ref="L14:P15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="K1:P2"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
@@ -2887,34 +2889,32 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="L14:P15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:P5"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="L8:P9"/>
+    <mergeCell ref="L10:P11"/>
+    <mergeCell ref="L12:P13"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new amp for Paul
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Input List.xlsx
+++ b/Input List/Full Band/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF33A14-259D-4353-B137-0899931A2717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13926E15-97C0-4E0E-AD05-7C3F6C8AAAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="174">
   <si>
     <t>Input</t>
   </si>
@@ -397,12 +397,6 @@
     <t>Drum 10</t>
   </si>
   <si>
-    <t>Drum 11</t>
-  </si>
-  <si>
-    <t>Drum 12</t>
-  </si>
-  <si>
     <t>DSR 1</t>
   </si>
   <si>
@@ -592,6 +586,21 @@
   </si>
   <si>
     <t>Full Band Setup</t>
+  </si>
+  <si>
+    <t>Behringer B906</t>
+  </si>
+  <si>
+    <t>USL 1</t>
+  </si>
+  <si>
+    <t>USL 2</t>
+  </si>
+  <si>
+    <t>USL 3</t>
+  </si>
+  <si>
+    <t>DSR 5</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1042,14 +1051,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1098,47 +1149,65 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1176,65 +1245,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1642,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,35 +1675,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="e" vm="1">
+      <c r="A1" s="52" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="24" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="24"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="25" t="str">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="40" t="str">
         <f ca="1">"Date Updated: "&amp;TEXT(TODAY(),"yyyy-mm-dd")</f>
-        <v>Date Updated: 2024-10-13</v>
-      </c>
-      <c r="I2" s="25"/>
+        <v>Date Updated: 2024-11-17</v>
+      </c>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1701,7 +1716,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>91</v>
@@ -1720,17 +1735,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="10">
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>96</v>
@@ -1749,13 +1764,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="47"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="11">
         <v>2</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>97</v>
@@ -1770,17 +1785,17 @@
         <v>26</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="10">
         <v>3</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>98</v>
@@ -1797,13 +1812,13 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="11">
         <v>4</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>99</v>
@@ -1818,17 +1833,17 @@
         <v>71</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="47"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="10">
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>100</v>
@@ -1843,17 +1858,17 @@
         <v>71</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="11">
         <v>6</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>101</v>
@@ -1868,17 +1883,17 @@
         <v>71</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="10">
         <v>7</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>102</v>
@@ -1893,17 +1908,17 @@
         <v>71</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="11">
         <v>8</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>103</v>
@@ -1918,17 +1933,17 @@
         <v>71</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="10">
         <v>9</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>104</v>
@@ -1943,17 +1958,17 @@
         <v>93</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="48"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="11">
         <v>10</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>105</v>
@@ -1968,7 +1983,7 @@
         <v>93</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,15 +1993,15 @@
         <v>11</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -1995,15 +2010,15 @@
         <v>12</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -2012,15 +2027,15 @@
         <v>13</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -2029,28 +2044,28 @@
         <v>14</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E17" s="12"/>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="51" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="13">
         <v>15</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>33</v>
@@ -2067,13 +2082,13 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="14">
         <v>16</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>33</v>
@@ -2090,20 +2105,20 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>151</v>
+      <c r="B20" s="47" t="s">
+        <v>149</v>
       </c>
       <c r="C20" s="15">
         <v>17</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>18</v>
@@ -2119,16 +2134,16 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="16">
         <v>18</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>19</v>
@@ -2142,16 +2157,16 @@
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="15">
         <v>19</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>52</v>
@@ -2165,20 +2180,20 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="50" t="s">
         <v>84</v>
       </c>
       <c r="C23" s="17">
         <v>20</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>43</v>
@@ -2190,20 +2205,20 @@
         <v>93</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="18">
         <v>21</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>51</v>
@@ -2217,20 +2232,20 @@
       <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="43" t="s">
         <v>85</v>
       </c>
       <c r="C25" s="19">
         <v>22</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>1</v>
@@ -2246,16 +2261,16 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="44"/>
       <c r="C26" s="20">
         <v>23</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>2</v>
@@ -2269,21 +2284,27 @@
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="12">
+      <c r="A27" s="88"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="19">
         <v>24</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
+      <c r="D27" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -2292,31 +2313,31 @@
         <v>25</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E28" s="12"/>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
     </row>
     <row r="29" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="53" t="s">
-        <v>152</v>
+      <c r="B29" s="36" t="s">
+        <v>150</v>
       </c>
       <c r="C29" s="21">
         <v>26</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>3</v>
@@ -2332,16 +2353,16 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="22">
         <v>27</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F30" s="22" t="s">
         <v>4</v>
@@ -2355,16 +2376,16 @@
       <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="21">
         <v>28</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>38</v>
@@ -2378,16 +2399,16 @@
       <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="54"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="22">
         <v>29</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="F32" s="22" t="s">
         <v>39</v>
@@ -2401,16 +2422,16 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="21">
         <v>30</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>40</v>
@@ -2424,17 +2445,17 @@
       <c r="I33" s="21"/>
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="32" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="13">
         <v>31</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>33</v>
@@ -2449,17 +2470,17 @@
         <v>76</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="14">
         <v>32</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>33</v>
@@ -2474,24 +2495,13 @@
         <v>76</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
+  <mergeCells count="23">
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="A23:A24"/>
@@ -2503,6 +2513,16 @@
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2514,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -2529,86 +2549,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="e" vm="1">
+      <c r="A1" s="52" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="40" t="str">
+      <c r="B1" s="52"/>
+      <c r="C1" s="54" t="str">
         <f>'Input + Equipment'!C1</f>
         <v>Full Band Setup</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="24" t="str">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="39" t="str">
         <f>'Input + Equipment'!H1</f>
         <v>www.theperfectstrangers.band</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="25" t="str">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="40" t="str">
         <f ca="1">'Input + Equipment'!H2</f>
-        <v>Date Updated: 2024-10-13</v>
-      </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+        <v>Date Updated: 2024-11-17</v>
+      </c>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="5"/>
-      <c r="K3" s="87" t="s">
+      <c r="K3" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="5"/>
-      <c r="K4" s="66">
+      <c r="K4" s="86">
         <v>1</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="57"/>
+      <c r="M4" s="77"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -2636,57 +2656,57 @@
         <v>8</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="59"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="79"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="70" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="K6" s="64">
+      <c r="K6" s="84">
         <v>2</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="61"/>
+      <c r="M6" s="81"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="74"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="71"/>
       <c r="I7" s="5"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="63"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="83"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -2698,13 +2718,13 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="5"/>
-      <c r="K8" s="66">
+      <c r="K8" s="86">
         <v>3</v>
       </c>
-      <c r="L8" s="56" t="s">
+      <c r="L8" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="57"/>
+      <c r="M8" s="77"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -2732,75 +2752,75 @@
         <v>16</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="59"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="79"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="75" t="s">
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="66" t="s">
         <v>78</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="K10" s="64">
+      <c r="K10" s="84">
         <v>4</v>
       </c>
-      <c r="L10" s="60" t="s">
+      <c r="L10" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="61"/>
+      <c r="M10" s="81"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="5"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="63"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="83"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="5"/>
-      <c r="K12" s="66">
+      <c r="K12" s="86">
         <v>5</v>
       </c>
-      <c r="L12" s="56" t="s">
+      <c r="L12" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="57"/>
+      <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="5"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="59"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="79"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -2828,49 +2848,49 @@
         <v>8</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="K14" s="64">
+      <c r="K14" s="84">
         <v>6</v>
       </c>
-      <c r="L14" s="60" t="s">
+      <c r="L14" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="M14" s="61"/>
+      <c r="M14" s="81"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
       <c r="I15" s="5"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="83"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2886,54 +2906,54 @@
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I18" s="5"/>
-      <c r="K18" s="86" t="s">
-        <v>169</v>
-      </c>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
+      <c r="K18" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="5"/>
       <c r="K19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="5"/>
       <c r="K20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2963,67 +2983,67 @@
       </c>
       <c r="I21" s="5"/>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="82" t="s">
+      <c r="F22" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="82" t="s">
+      <c r="G22" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="68"/>
+      <c r="H22" s="63"/>
       <c r="I22" s="5"/>
       <c r="K22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="68"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="63"/>
       <c r="I23" s="5"/>
       <c r="K23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3037,13 +3057,13 @@
       <c r="H24" s="7"/>
       <c r="I24" s="5"/>
       <c r="K24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,55 +3094,55 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="80" t="s">
+      <c r="A26" s="68"/>
+      <c r="B26" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="80" t="s">
+      <c r="E26" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="80" t="s">
+      <c r="F26" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="75" t="s">
+      <c r="G26" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="75" t="s">
+      <c r="H26" s="66" t="s">
         <v>75</v>
       </c>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3153,39 +3173,39 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="84" t="s">
+      <c r="D31" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="85" t="s">
+      <c r="E31" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="68"/>
-      <c r="G31" s="83" t="s">
+      <c r="F31" s="63"/>
+      <c r="G31" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="83" t="s">
+      <c r="H31" s="58" t="s">
         <v>61</v>
       </c>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3195,33 +3215,35 @@
     <row r="35" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="L4:M5"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L10:M11"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -3238,35 +3260,33 @@
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="L4:M5"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L10:M11"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>